<commit_message>
Update Tableau concurrant pp45.xlsx
</commit_message>
<xml_diff>
--- a/Nelson GRAVEAU/Tableau concurrant pp45.xlsx
+++ b/Nelson GRAVEAU/Tableau concurrant pp45.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelson\Documents\GitHub\SN2_SFL4Manitou_23\Nelson GRAVEAU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4BF17186-3E62-42FB-B62A-1E489C489DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE06A95-5C71-4B7C-B1EF-466A05392B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{13CE86CE-D830-4741-8F26-49317392E8DB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Rockwell Automation</t>
   </si>
@@ -66,12 +66,6 @@
   </si>
   <si>
     <t>TP 177A</t>
-  </si>
-  <si>
-    <t>Site</t>
-  </si>
-  <si>
-    <t>wiautomation.com</t>
   </si>
   <si>
     <t>Prix (HT)</t>
@@ -104,7 +98,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -127,11 +121,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -139,7 +155,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -553,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60AFAB47-3746-445E-BAF2-DFCA100D37E9}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -565,7 +588,7 @@
     <col min="2" max="3" width="31.88671875" customWidth="1"/>
     <col min="4" max="4" width="65.5546875" customWidth="1"/>
     <col min="5" max="5" width="13.109375" customWidth="1"/>
-    <col min="6" max="6" width="21" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -579,14 +602,12 @@
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -597,12 +618,10 @@
         <v>9</v>
       </c>
       <c r="D2" s="1"/>
-      <c r="E2" s="3">
+      <c r="E2" s="4">
         <v>850</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -611,8 +630,8 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -621,8 +640,8 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -631,8 +650,8 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -641,8 +660,8 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -651,10 +670,22 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="3">
+      <c r="E7" s="4">
         <v>400</v>
       </c>
-      <c r="F7" s="1"/>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F11" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
tableau concurrent petite modif
</commit_message>
<xml_diff>
--- a/Nelson GRAVEAU/Tableau concurrant pp45.xlsx
+++ b/Nelson GRAVEAU/Tableau concurrant pp45.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelson\Documents\GitHub\SN2_SFL4Manitou_23\Nelson GRAVEAU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5046793D-6D4F-4AF2-BA09-6E45D6BBBFC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A676C5-02A7-445E-B826-B258AC4AE33C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{13CE86CE-D830-4741-8F26-49317392E8DB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Rockwell Automation</t>
   </si>
@@ -316,17 +316,32 @@
 Protection : IP65 (face avant) / IP20 (panneau arriere)</t>
   </si>
   <si>
-    <t>processeur : de 350 MHz à 1 GHz</t>
+    <t>processeur : de 350 MHz à 1 GHz
+RAM: 256 MB 
+Diagonales : 5,7 pouces
+résolution : 320 x 240px
+Dimensions (L x H x P) : 185 x 152 x 68mm
+Couleurs : N/A
+Type d'affichage : TFT
+Poids : 594
+Protection :	IP66 (face avant)</t>
+  </si>
+  <si>
+    <t>processeur : MRA
+Flash / RAM : 512 kbyte
+Diagonales : 5,7 pouces
+résolution : 320 x 240px
+Dimensions (L x H x P) : 212 x 156 x 44 mm 
+Couleurs : 2
+Type d'affichage : LCD
+Poids : 0,75 kg
+Protection : IP65 (face avant) / IP20 (panneau arriere)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="6" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
-    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -430,7 +445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -457,18 +472,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1065,8 +1071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60AFAB47-3746-445E-BAF2-DFCA100D37E9}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1074,7 +1080,7 @@
     <col min="1" max="1" width="19.88671875" customWidth="1"/>
     <col min="2" max="4" width="31.88671875" customWidth="1"/>
     <col min="5" max="5" width="65.5546875" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" customWidth="1"/>
     <col min="7" max="7" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1110,8 +1116,10 @@
       <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="11">
+      <c r="E2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="10">
         <v>850</v>
       </c>
       <c r="G2" s="3"/>
@@ -1129,7 +1137,7 @@
       <c r="E3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="10">
         <v>2600</v>
       </c>
       <c r="G3" s="3"/>
@@ -1145,10 +1153,10 @@
       <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="10">
         <v>1465.56</v>
       </c>
       <c r="G4" s="3"/>
@@ -1163,10 +1171,10 @@
       <c r="D5" s="1">
         <v>288037</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="10">
         <v>1409.54</v>
       </c>
       <c r="G5" s="3"/>
@@ -1182,10 +1190,10 @@
       <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="10">
         <v>400</v>
       </c>
       <c r="G6" s="3"/>

</xml_diff>